<commit_message>
Data in Excel sheet
Added invoice values to the excel sheet in Frame2
</commit_message>
<xml_diff>
--- a/MyProject/test.xlsx
+++ b/MyProject/test.xlsx
@@ -99,7 +99,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -312,6 +312,12 @@
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -346,7 +352,7 @@
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true"/>
   </cellXfs>
 </styleSheet>
 </file>

</xml_diff>

<commit_message>
fixed the bugs Frame3 done
new frame to add the final touches
</commit_message>
<xml_diff>
--- a/MyProject/test.xlsx
+++ b/MyProject/test.xlsx
@@ -424,33 +424,36 @@
         <v>1.0</v>
       </c>
       <c r="B5" t="n">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="C5" t="n">
-        <v>23.0</v>
+        <v>0.0</v>
       </c>
       <c r="D5" t="n">
-        <v>34.0</v>
+        <v>0.0</v>
       </c>
       <c r="E5" t="n">
-        <v>45.0</v>
+        <v>0.0</v>
       </c>
       <c r="F5" t="n">
-        <v>65.0</v>
+        <v>0.0</v>
       </c>
       <c r="G5" t="n">
-        <v>67.0</v>
+        <v>0.0</v>
       </c>
       <c r="H5" t="n">
-        <v>86.0</v>
+        <v>0.0</v>
       </c>
       <c r="I5" t="n">
-        <v>858.0</v>
+        <v>0.0</v>
       </c>
       <c r="J5" t="n">
-        <v>97.0</v>
+        <v>0.0</v>
       </c>
       <c r="K5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L5" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -459,34 +462,37 @@
         <v>2.0</v>
       </c>
       <c r="B6" t="n">
-        <v>9.0</v>
+        <v>15.0</v>
       </c>
       <c r="C6" t="n">
-        <v>98.0</v>
+        <v>10.0</v>
       </c>
       <c r="D6" t="n">
-        <v>87.0</v>
+        <v>1500.0</v>
       </c>
       <c r="E6" t="n">
-        <v>76.0</v>
+        <v>100000.0</v>
       </c>
       <c r="F6" t="n">
-        <v>65.0</v>
+        <v>10.0</v>
       </c>
       <c r="G6" t="n">
-        <v>45.0</v>
+        <v>10.0</v>
       </c>
       <c r="H6" t="n">
-        <v>43.0</v>
+        <v>10.0</v>
       </c>
       <c r="I6" t="n">
-        <v>32.0</v>
+        <v>80.0</v>
       </c>
       <c r="J6" t="n">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="K6" t="n">
-        <v>23.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>100100.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculation commit with frame4
added calculations(still have to add) made a vba and made a custom formula ..
</commit_message>
<xml_diff>
--- a/MyProject/test.xlsx
+++ b/MyProject/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>test</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>CGST</t>
+  </si>
+  <si>
+    <t>SGST</t>
   </si>
 </sst>
 </file>
@@ -58,13 +70,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -323,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="true" applyFont="true">
       <alignment horizontal="center" vertical="center"/>
@@ -353,13 +370,15 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A3:L6"/>
+  <dimension ref="A3:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -420,79 +439,95 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="n" s="9">
         <v>1.0</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="n" s="9">
+        <v>100.0</v>
+      </c>
+      <c r="C5" t="n" s="9">
+        <v>1500.0</v>
+      </c>
+      <c r="D5" t="n" s="9">
         <v>0.0</v>
       </c>
-      <c r="C5" t="n">
+      <c r="E5" t="n" s="9">
         <v>0.0</v>
       </c>
-      <c r="D5" t="n">
+      <c r="F5" t="n" s="9">
+        <v>150.0</v>
+      </c>
+      <c r="G5" t="n" s="9">
+        <v>250.0</v>
+      </c>
+      <c r="H5" t="n" s="9">
         <v>0.0</v>
       </c>
-      <c r="E5" t="n">
+      <c r="I5" t="n" s="9">
         <v>0.0</v>
       </c>
-      <c r="F5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B6" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1500.0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>100000.0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>100100.0</v>
+      <c r="J5" t="n" s="9">
+        <v>150.0</v>
+      </c>
+      <c r="K5" t="n" s="9">
+        <v>250.0</v>
+      </c>
+      <c r="L5" t="n" s="9">
+        <v>2000.0</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" t="s" s="10">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s" s="10">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s" s="10">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s" s="10">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s" s="10">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="J7" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="K7" t="s" s="10">
+        <v>11</v>
+      </c>
+      <c r="L7" t="s" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="10">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>